<commit_message>
[FIX] Make it runnable, switch pdf engine => requires libreoffice on the machine
</commit_message>
<xml_diff>
--- a/example/registration/registration.xlsx
+++ b/example/registration/registration.xlsx
@@ -166,7 +166,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -187,17 +187,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -415,16 +404,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -444,18 +429,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,59 +448,59 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -535,11 +516,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -563,10 +552,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -579,15 +564,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -606,19 +595,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="2.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="3.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="1" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="2.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="2.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="3.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,198 +686,207 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6" t="s">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="9" t="s">
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="11" t="s">
+      <c r="K7" s="8"/>
+      <c r="L7" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="16"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="17" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="16"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="L11" s="22"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="21"/>
+      <c r="J11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="22" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="H12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>26</v>
-      </c>
+      <c r="A12" s="10"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="25" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="25" t="s">
+      <c r="H13" s="24"/>
+      <c r="I13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="26"/>
-      <c r="K13" s="25" t="s">
+      <c r="J13" s="24"/>
+      <c r="K13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="27"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="32"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="22"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="32"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="33" t="s">
         <v>36</v>
       </c>
@@ -901,111 +903,111 @@
       <c r="H16" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="39" t="s">
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="38" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="33"/>
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
       <c r="F17" s="35"/>
       <c r="G17" s="35"/>
       <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="39"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="38"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="40" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="22"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="32"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="40" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="22"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="41" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="27"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16"/>
-      <c r="L21" s="22"/>
+      <c r="A21" s="14"/>
+      <c r="L21" s="32"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16"/>
-      <c r="L22" s="22"/>
+      <c r="A22" s="14"/>
+      <c r="L22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16"/>
-      <c r="L23" s="22"/>
+      <c r="A23" s="14"/>
+      <c r="L23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16"/>
-      <c r="L24" s="22"/>
+      <c r="A24" s="14"/>
+      <c r="L24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16"/>
-      <c r="L25" s="22"/>
+      <c r="A25" s="14"/>
+      <c r="L25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="42"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
       <c r="L26" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="38">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:I4"/>
     <mergeCell ref="B5:K5"/>
@@ -1024,6 +1026,12 @@
     <mergeCell ref="G10:L10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:F13"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
     <mergeCell ref="A14:B20"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:E15"/>

</xml_diff>

<commit_message>
[ADD] Form fillup feature (#14)
* [ADD] Form Producer / Change markup stucture

* [WIP] Add fillup processing/pdf export

* [WIP] Adjust coroutines to create chain excel_fill->pdf export

* [WIP] Testing solution

* [WIP] Bugfixes

* [FIX] Make it runnable, switch pdf engine => requires libreoffice on the machine

* [MERGE]

* [CONFIG] Gitignore

* Add formproc processing to template controller

---------

Co-authored-by: V.Kuznetsov <izy@youmu.ru>
Co-authored-by: Savva Frolenko <s.frolenko@betby.com>
</commit_message>
<xml_diff>
--- a/example/registration/registration.xlsx
+++ b/example/registration/registration.xlsx
@@ -166,7 +166,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -187,17 +187,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -415,16 +404,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -444,18 +429,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,59 +448,59 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -535,11 +516,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -563,10 +552,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -579,15 +564,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -606,19 +595,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="2.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="3.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="1" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="2.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="2.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="3.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,198 +686,207 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6" t="s">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="9" t="s">
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="11" t="s">
+      <c r="K7" s="8"/>
+      <c r="L7" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="16"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="17" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="16"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="L11" s="22"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="21"/>
+      <c r="J11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="22" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="H12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>26</v>
-      </c>
+      <c r="A12" s="10"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="25" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="25" t="s">
+      <c r="H13" s="24"/>
+      <c r="I13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="26"/>
-      <c r="K13" s="25" t="s">
+      <c r="J13" s="24"/>
+      <c r="K13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="27"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="32"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="22"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="32"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="33" t="s">
         <v>36</v>
       </c>
@@ -901,111 +903,111 @@
       <c r="H16" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="39" t="s">
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="38" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="33"/>
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
       <c r="F17" s="35"/>
       <c r="G17" s="35"/>
       <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="39"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="38"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="40" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="22"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="32"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="40" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="22"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="41" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="27"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16"/>
-      <c r="L21" s="22"/>
+      <c r="A21" s="14"/>
+      <c r="L21" s="32"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16"/>
-      <c r="L22" s="22"/>
+      <c r="A22" s="14"/>
+      <c r="L22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16"/>
-      <c r="L23" s="22"/>
+      <c r="A23" s="14"/>
+      <c r="L23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16"/>
-      <c r="L24" s="22"/>
+      <c r="A24" s="14"/>
+      <c r="L24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16"/>
-      <c r="L25" s="22"/>
+      <c r="A25" s="14"/>
+      <c r="L25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="42"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
       <c r="L26" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="38">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:I4"/>
     <mergeCell ref="B5:K5"/>
@@ -1024,6 +1026,12 @@
     <mergeCell ref="G10:L10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:F13"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
     <mergeCell ref="A14:B20"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:E15"/>

</xml_diff>

<commit_message>
[HOT] Mark in XLSX and test pdf export
</commit_message>
<xml_diff>
--- a/example/registration/registration.xlsx
+++ b/example/registration/registration.xlsx
@@ -399,7 +399,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -429,7 +429,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -482,10 +482,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -599,8 +595,8 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -714,7 +710,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="24.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -806,12 +802,12 @@
       <c r="H11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="21"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="21"/>
-      <c r="L11" s="22" t="s">
+      <c r="K11" s="20"/>
+      <c r="L11" s="21" t="s">
         <v>26</v>
       </c>
     </row>
@@ -824,10 +820,10 @@
       <c r="F12" s="19"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="22"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10"/>
@@ -836,175 +832,175 @@
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="23" t="s">
+      <c r="H13" s="23"/>
+      <c r="I13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="24"/>
-      <c r="K13" s="23" t="s">
+      <c r="J13" s="23"/>
+      <c r="K13" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="25"/>
+      <c r="L13" s="24"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="31"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="32"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="31"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="33" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="35" t="s">
+      <c r="E16" s="33"/>
+      <c r="F16" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H16" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="38" t="s">
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="37" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="38"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="37"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="39" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="32"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="39" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="32"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="31"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="40" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="25"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14"/>
-      <c r="L21" s="32"/>
+      <c r="L21" s="31"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14"/>
-      <c r="L22" s="32"/>
+      <c r="L22" s="31"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14"/>
-      <c r="L23" s="32"/>
+      <c r="L23" s="31"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14"/>
-      <c r="L24" s="32"/>
+      <c r="L24" s="31"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14"/>
-      <c r="L25" s="32"/>
+      <c r="L25" s="31"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="44"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="38">

</xml_diff>